<commit_message>
corrigido bug contagem pontos por títulos
Identificado e corrigido bug na contagem de pontos por títulos
</commit_message>
<xml_diff>
--- a/data/Nova pasta/ArquivoTitulos.xlsx
+++ b/data/Nova pasta/ArquivoTitulos.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\GitHub\GOAT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\GitHub\GOAT\data\Nova pasta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17025" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="CR" sheetId="2" r:id="rId1"/>
-    <sheet name="Messi" sheetId="4" r:id="rId2"/>
+    <sheet name="Títulos" sheetId="2" r:id="rId1"/>
+    <sheet name="CR" sheetId="5" r:id="rId2"/>
+    <sheet name="Messi" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="136">
   <si>
     <t>3X MELHOR JOGADOR DO MUNDO</t>
   </si>
@@ -36,21 +37,9 @@
     <t>Manchester United FC</t>
   </si>
   <si>
-    <t>5X VENCEDOR BALLON D'OR</t>
-  </si>
-  <si>
-    <t>4X O FUTEBOLISTA DO ANO DA EUROPA</t>
-  </si>
-  <si>
-    <t>10X FUTEBOLISTA DO ANO</t>
-  </si>
-  <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t>19X MELHOR MARCADOR</t>
-  </si>
-  <si>
     <t>20/21</t>
   </si>
   <si>
@@ -76,9 +65,6 @@
   </si>
   <si>
     <t>FA Cup</t>
-  </si>
-  <si>
-    <t>2X FUTEBOLISTA DO ANO (TRANSFERMARKT.DE ESCOLHA DO UTILIZADOR)</t>
   </si>
   <si>
     <t>Itália</t>
@@ -531,6 +517,99 @@
   </si>
   <si>
     <t>Lionel Messi</t>
+  </si>
+  <si>
+    <t>JOGADOR</t>
+  </si>
+  <si>
+    <t>MELHOR JOGADOR DO MUNDO</t>
+  </si>
+  <si>
+    <t>VENCEDOR BALLON D'OR</t>
+  </si>
+  <si>
+    <t>O FUTEBOLISTA DO ANO DA EUROPA</t>
+  </si>
+  <si>
+    <t>FUTEBOLISTA DO ANO</t>
+  </si>
+  <si>
+    <t>MELHOR MARCADOR</t>
+  </si>
+  <si>
+    <t>FUTEBOLISTA DO ANO (TRANSFERMARKT.DE ESCOLHA DO UTILIZADOR)</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DA EUROPA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA CHAMPIONS-LEAGUE</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DO MUNDO FIFA-KLUB</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DA INGLATERRA</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DE ESPANHA</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DE ITÁLIA</t>
+  </si>
+  <si>
+    <t>VENCEDOR UEFA NATIONS LEAGUE</t>
+  </si>
+  <si>
+    <t>VENCEDOR UEFA-SUPERCUP</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA TAÇA DE INGLATERRA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA TAÇA DE ESPANHA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA TAÇA DE ITÁLIA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA TAÇA DA LIGA DE INGLATERRA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA SUPERTAÇA DE ESPANHA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA SUPERTAÇA DA ITÁLIA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA SUPERTAÇA DE INGLATERRA</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA SUPERTAÇA DE PORTUGAL</t>
+  </si>
+  <si>
+    <t>VENCEDOR BALLON D OR</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DO MUNDO</t>
+  </si>
+  <si>
+    <t>VENCEDOR COPA AMÉRICA</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DE FRANÇA</t>
+  </si>
+  <si>
+    <t>CAMPEÃO DO MUNDO SUB20</t>
+  </si>
+  <si>
+    <t>CONMEBOL-UEFA CUP OF CHAMPIONS WINNER</t>
+  </si>
+  <si>
+    <t>VENCEDOR DA SUPERTAÇA DE FRANÇA</t>
+  </si>
+  <si>
+    <t>VENCEDOR OLÍMPICO</t>
   </si>
 </sst>
 </file>
@@ -637,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -701,6 +780,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -992,23 +1086,27 @@
     <col min="1" max="1" width="44.28515625" style="15" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" style="13" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="36.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="37.5">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="B2" s="5">
         <v>2017</v>
@@ -1016,10 +1114,13 @@
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
-        <v>0</v>
+      <c r="D2" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="B3" s="5">
         <v>2016</v>
@@ -1027,10 +1128,13 @@
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="14" t="s">
-        <v>0</v>
+      <c r="D3" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="B4" s="5">
         <v>2008</v>
@@ -1038,65 +1142,83 @@
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="14" t="s">
-        <v>3</v>
+      <c r="D4" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="B5" s="5">
         <v>2017</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="14" t="s">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="B6" s="5">
         <v>2016</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="14" t="s">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="B7" s="5">
         <v>2014</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="14" t="s">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="B8" s="5">
         <v>2013</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="14" t="s">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="B9" s="5">
         <v>2008</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="14" t="s">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="B10" s="5">
         <v>2017</v>
@@ -1104,10 +1226,13 @@
       <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="14" t="s">
-        <v>4</v>
+      <c r="D10" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="B11" s="5">
         <v>2016</v>
@@ -1115,10 +1240,13 @@
       <c r="C11" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="14" t="s">
-        <v>4</v>
+      <c r="D11" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="B12" s="5">
         <v>2014</v>
@@ -1126,10 +1254,13 @@
       <c r="C12" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="14" t="s">
-        <v>4</v>
+      <c r="D12" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="B13" s="5">
         <v>2008</v>
@@ -1137,417 +1268,531 @@
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="14" t="s">
-        <v>5</v>
+      <c r="D13" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B14" s="5">
         <v>2018</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B15" s="5">
         <v>2017</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B16" s="5">
         <v>2016</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B17" s="5">
         <v>2015</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B18" s="5">
         <v>2013</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B19" s="5">
         <v>2012</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B20" s="5">
         <v>2011</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B21" s="5">
         <v>2009</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B22" s="5">
         <v>2008</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B23" s="5">
         <v>2007</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1">
+      <c r="A24" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30">
+      <c r="A26" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1">
-      <c r="A24" s="14" t="s">
+      <c r="C27" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="D27" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="D30" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="30">
-      <c r="A26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="D31" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="D32" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="C34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="27">
+      <c r="A37" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="27">
-      <c r="A37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="28.5">
-      <c r="A43" s="14" t="s">
-        <v>17</v>
+      <c r="D42" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="42.75">
+      <c r="A43" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="B43" s="8">
         <v>2019</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="28.5">
-      <c r="A44" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="42.75">
+      <c r="A44" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="B44" s="8">
         <v>2017</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="14" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="B45" s="8">
         <v>2016</v>
       </c>
       <c r="C45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="14" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="14" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1">
+      <c r="D48" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="14" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1">
+      <c r="D49" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1">
+      <c r="D50" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="14" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="B51" s="8">
         <v>2017</v>
@@ -1555,10 +1800,13 @@
       <c r="C51" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
+      <c r="D51" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="14" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="B52" s="8">
         <v>2016</v>
@@ -1566,10 +1814,13 @@
       <c r="C52" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
+      <c r="D52" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="14" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="B53" s="8">
         <v>2014</v>
@@ -1577,10 +1828,13 @@
       <c r="C53" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1">
+      <c r="D53" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="14" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="B54" s="8">
         <v>2008</v>
@@ -1588,10 +1842,13 @@
       <c r="C54" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1">
+      <c r="D54" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="14" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="B55" s="8">
         <v>2009</v>
@@ -1599,10 +1856,13 @@
       <c r="C55" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1">
+      <c r="D55" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="14" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="B56" s="8">
         <v>2008</v>
@@ -1610,10 +1870,13 @@
       <c r="C56" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1">
+      <c r="D56" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="B57" s="8">
         <v>2007</v>
@@ -1621,21 +1884,27 @@
       <c r="C57" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1">
+      <c r="D57" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1">
+      <c r="D58" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="14" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="B59" s="9">
         <v>45271</v>
@@ -1643,76 +1912,97 @@
       <c r="C59" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="14" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="14" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1">
+        <v>22</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="B62" s="8">
         <v>2019</v>
       </c>
       <c r="C62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" customHeight="1">
+      <c r="A63" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1">
-      <c r="A63" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="15" customHeight="1">
+      <c r="D63" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="14" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1">
+      <c r="D64" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="14" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1">
+      <c r="D65" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="B66" s="8">
         <v>2004</v>
@@ -1720,43 +2010,55 @@
       <c r="C66" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="15" customHeight="1">
+      <c r="D66" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="14" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1">
+      <c r="D67" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="14" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1">
+      <c r="D68" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="14" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="28.5">
+        <v>22</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="28.5">
       <c r="A70" s="14" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="B70" s="8">
         <v>2009</v>
@@ -1764,10 +2066,13 @@
       <c r="C70" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="28.5">
+      <c r="D70" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="28.5">
       <c r="A71" s="14" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="B71" s="8">
         <v>2006</v>
@@ -1775,54 +2080,69 @@
       <c r="C71" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="28.5">
+      <c r="D71" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="28.5">
       <c r="A72" s="14" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="28.5">
+      <c r="D72" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="28.5">
       <c r="A73" s="14" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="14" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15" customHeight="1">
+        <v>22</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="28.5">
+        <v>22</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="28.5">
       <c r="A76" s="14" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B76" s="8">
         <v>2008</v>
@@ -1830,10 +2150,13 @@
       <c r="C76" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="28.5">
+      <c r="D76" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="28.5">
       <c r="A77" s="14" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B77" s="8">
         <v>2007</v>
@@ -1841,16 +2164,1156 @@
       <c r="C77" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="28.5">
+      <c r="D77" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="28.5">
       <c r="A78" s="14" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="B78" s="8">
         <v>2002</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="17">
+        <v>2019</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D80" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" s="17">
+        <v>2009</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" s="17">
+        <v>2019</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D83" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" s="17">
+        <v>2015</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" s="17">
+        <v>2012</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" s="17">
+        <v>2011</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="17">
+        <v>2010</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="17">
+        <v>2009</v>
+      </c>
+      <c r="C88" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="17">
+        <v>2015</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B90" s="17">
+        <v>2011</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D90" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B91" s="17">
+        <v>2009</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D93" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D100" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D101" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D102" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C104" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D105" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B106" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D107" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D109" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D110" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C111" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D111" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C112" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="24">
+      <c r="A113" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B113" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C113" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D113" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="42.75">
+      <c r="A114" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B114" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="42.75">
+      <c r="A115" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B115" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C115" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="42.75">
+      <c r="A116" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B116" s="17">
+        <v>2019</v>
+      </c>
+      <c r="C116" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="42.75">
+      <c r="A117" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B117" s="17">
+        <v>2018</v>
+      </c>
+      <c r="C117" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B118" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C118" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D118" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B119" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D119" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B120" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D120" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D121" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B122" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C122" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D122" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B123" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D123" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B124" s="19">
+        <v>2016</v>
+      </c>
+      <c r="C124" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D124" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B125" s="19">
+        <v>2012</v>
+      </c>
+      <c r="C125" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D125" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B126" s="19">
+        <v>2010</v>
+      </c>
+      <c r="C126" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D126" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B127" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D127" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B128" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D128" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B129" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D129" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B130" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D130" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B131" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D131" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B132" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C132" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D132" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B133" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C133" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D133" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B134" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C134" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D134" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B135" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C135" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D135" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B136" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C136" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D136" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B137" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C137" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D137" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B138" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D138" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B139" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C139" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D139" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B140" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C140" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D140" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B141" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D141" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B142" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D142" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B143" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D143" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B144" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D144" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B145" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D145" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B146" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C146" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D146" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D147" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="28.5">
+      <c r="A148" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B148" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D148" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="28.5">
+      <c r="A149" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B149" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D149" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="28.5">
+      <c r="A150" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B150" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D150" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="28.5">
+      <c r="A151" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B151" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D151" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="28.5">
+      <c r="A152" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B152" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D152" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="28.5">
+      <c r="A153" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B153" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C153" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D153" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="28.5">
+      <c r="A154" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B154" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C154" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D154" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="28.5">
+      <c r="A155" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B155" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C155" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D155" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B156" s="20">
+        <v>2005</v>
+      </c>
+      <c r="C156" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D156" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="28.5">
+      <c r="A157" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B157" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C157" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D157" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B158" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C158" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D158" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B159" s="21">
+        <v>45177</v>
+      </c>
+      <c r="C159" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D159" s="29" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1863,10 +3326,888 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C78"/>
+  <sheetViews>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D43" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.28515625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="26">
+        <v>2017</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="26">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="26">
+        <v>2008</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="26">
+        <v>2017</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="26">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="26">
+        <v>2014</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="26">
+        <v>2013</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="26">
+        <v>2008</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="26">
+        <v>2017</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="26">
+        <v>2016</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="26">
+        <v>2014</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="26">
+        <v>2008</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="26">
+        <v>2018</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="26">
+        <v>2017</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="26">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="26">
+        <v>2015</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="26">
+        <v>2013</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="26">
+        <v>2012</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="26">
+        <v>2011</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="26">
+        <v>2009</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="26">
+        <v>2008</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="26">
+        <v>2007</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="27">
+      <c r="A26" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="42.75">
+      <c r="A43" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="27">
+        <v>2019</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="42.75">
+      <c r="A44" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="27">
+        <v>2017</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="8">
+        <v>2016</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="28.5">
+      <c r="A46" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="28.5">
+      <c r="A47" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="28.5">
+      <c r="A48" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="28.5">
+      <c r="A49" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="28.5">
+      <c r="A50" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="8">
+        <v>2017</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="8">
+        <v>2016</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="8">
+        <v>2014</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="8">
+        <v>2008</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="8">
+        <v>2009</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="8">
+        <v>2008</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="8">
+        <v>2007</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="9">
+        <v>45271</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="28.5">
+      <c r="A62" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="8">
+        <v>2019</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="28.5">
+      <c r="A66" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" s="8">
+        <v>2004</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="28.5">
+      <c r="A70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="8">
+        <v>2009</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="28.5">
+      <c r="A71" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" s="8">
+        <v>2006</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="28.5">
+      <c r="A72" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="28.5">
+      <c r="A73" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="28.5">
+      <c r="A74" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="28.5">
+      <c r="A75" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="28.5">
+      <c r="A76" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="8">
+        <v>2008</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="28.5">
+      <c r="A77" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="8">
+        <v>2007</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="28.5">
+      <c r="A78" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" s="8">
+        <v>2002</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C14"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1879,13 +4220,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="18.75">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1896,7 +4237,7 @@
         <v>2022</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1">
@@ -1907,7 +4248,7 @@
         <v>2019</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
@@ -1918,865 +4259,865 @@
         <v>2009</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B5" s="17">
         <v>2021</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B6" s="17">
         <v>2019</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B7" s="17">
         <v>2015</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B8" s="17">
         <v>2012</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B9" s="17">
         <v>2011</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B10" s="17">
         <v>2010</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B11" s="17">
         <v>2009</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.5">
       <c r="A12" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B12" s="17">
         <v>2015</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.5">
       <c r="A13" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B13" s="17">
         <v>2011</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.5">
       <c r="A14" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B14" s="17">
         <v>2009</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24">
       <c r="A19" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24">
       <c r="A24" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="24">
       <c r="A27" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="24">
       <c r="A30" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24">
       <c r="A33" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24">
       <c r="A35" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="24">
       <c r="A36" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="42.75">
       <c r="A37" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B37" s="17">
         <v>2021</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="42.75">
       <c r="A38" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B38" s="17">
         <v>2020</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="42.75">
       <c r="A39" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B39" s="17">
         <v>2019</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="42.75">
       <c r="A40" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B40" s="17">
         <v>2018</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B41" s="19">
         <v>2022</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="28.5">
       <c r="A43" s="16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="28.5">
       <c r="A44" s="16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="28.5">
       <c r="A45" s="16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.5">
       <c r="A46" s="16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B47" s="19">
         <v>2016</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B48" s="19">
         <v>2012</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B49" s="19">
         <v>2010</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="28.5">
       <c r="A71" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="28.5">
       <c r="A72" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="28.5">
       <c r="A73" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="28.5">
       <c r="A74" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="28.5">
       <c r="A75" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="28.5">
       <c r="A76" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.5">
       <c r="A77" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="28.5">
       <c r="A78" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B79" s="20">
         <v>2005</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="28.5">
       <c r="A80" s="16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="28.5">
       <c r="A81" s="16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B82" s="21">
         <v>45177</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>